<commit_message>
Actualización de clase couting
</commit_message>
<xml_diff>
--- a/src/site/resources/PSP1/psp forms/Size Estimating Templat.xlsx
+++ b/src/site/resources/PSP1/psp forms/Size Estimating Templat.xlsx
@@ -12,10 +12,10 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
-    <sheet name="excel (3)" sheetId="1" r:id="rId1"/>
+    <sheet name="excel (4)" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="excel__3" localSheetId="0">'excel (3)'!$A$1:$L$53</definedName>
+    <definedName name="excel__4" localSheetId="0">'excel (4)'!$A$1:$L$53</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -23,7 +23,7 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" odcFile="C:\Users\fbenavides\Downloads\excel (3).iqy" name="excel (3)" type="4" refreshedVersion="5" background="1" saveData="1">
+  <connection id="1" odcFile="C:\Users\fbenavides\Downloads\excel (4).iqy" name="excel (4)" type="4" refreshedVersion="5" background="1" saveData="1">
     <webPr consecutive="1" xl2000="1" url="http://localhost:2468/reports/form2html.class?uri=%2FNon%2BProject%2FPSP%2BFundamentals%2B%2526%2BAdvanced%2FProgram%2B2%2F%2Fpsp1%2Fsizeest%2Eclass&amp;EXPORT=excel" htmlFormat="all"/>
   </connection>
 </connections>
@@ -1263,7 +1263,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="excel (3)" preserveFormatting="0" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="excel (4)" preserveFormatting="0" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1820,7 +1820,7 @@
         <v>29</v>
       </c>
       <c r="K17" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L17" s="6"/>
     </row>
@@ -1876,7 +1876,7 @@
         <v>70</v>
       </c>
       <c r="K19" s="6">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="L19" s="6"/>
     </row>
@@ -1924,7 +1924,7 @@
         <v>37</v>
       </c>
       <c r="K21" s="6">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="L21" s="6"/>
     </row>
@@ -2347,10 +2347,10 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" display="http://localhost:2468/psp-lib/sizeinst.htm"/>
-    <hyperlink ref="A13" r:id="rId2" display="http://localhost:2468/reports/sizeest.class?moreBaseParts=6"/>
+    <hyperlink ref="A13" r:id="rId2" display="http://localhost:2468/reports/sizeest.class?moreBaseParts=3"/>
     <hyperlink ref="D15" r:id="rId3" display="http://localhost:2468/dash/sizePerItemEdit"/>
-    <hyperlink ref="A23" r:id="rId4" display="http://localhost:2468/reports/sizeest.class?moreNew=6"/>
-    <hyperlink ref="A27" r:id="rId5" display="http://localhost:2468/reports/sizeest.class?moreReused=6"/>
+    <hyperlink ref="A23" r:id="rId4" display="http://localhost:2468/reports/sizeest.class?moreNew=3"/>
+    <hyperlink ref="A27" r:id="rId5" display="http://localhost:2468/reports/sizeest.class?moreReused=3"/>
     <hyperlink ref="A31" r:id="rId6" display="http://localhost:2468/reports/probe/probe.class"/>
     <hyperlink ref="A49" r:id="rId7" display="http://localhost:2468/reports/probe/probe.class?page=report"/>
   </hyperlinks>

</xml_diff>